<commit_message>
data input u/ SumSel
</commit_message>
<xml_diff>
--- a/_DB/data/Sulawesi_Selatan/Buiding LDMProp.xlsx
+++ b/_DB/data/Sulawesi_Selatan/Buiding LDMProp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icrafguest01\tin\pprk_apps_tinbaru\aksara_rancang\_DB\data\Sulawesi_Selatan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56325098-8157-4FDF-A764-1639CE7C6A28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0F6364-45B8-4852-9C5A-5A0E5708611A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4BAF162A-D205-41CE-ABBA-C7F5AB9C6C07}"/>
+    <workbookView minimized="1" xWindow="2685" yWindow="945" windowWidth="13620" windowHeight="10920" xr2:uid="{4BAF162A-D205-41CE-ABBA-C7F5AB9C6C07}"/>
   </bookViews>
   <sheets>
     <sheet name="LDMProp" sheetId="1" r:id="rId1"/>
@@ -993,11 +993,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505F1DED-74C0-448A-93A2-D87C0E69031A}">
   <dimension ref="A1:X116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M1:O1048576"/>
+      <selection pane="bottomRight" activeCell="Y114" sqref="Y114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,6 +1005,7 @@
     <col min="1" max="1" width="61" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" customWidth="1"/>
   </cols>
@@ -9580,7 +9581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACA0FAC-721D-4557-962D-3E7FDB35651A}">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E114"/>
     </sheetView>
   </sheetViews>

</xml_diff>